<commit_message>
Added weekly heatmap, making heatmaps more stable with additional data transformations
</commit_message>
<xml_diff>
--- a/chartsFolder/scores.xlsx
+++ b/chartsFolder/scores.xlsx
@@ -383,2456 +383,2450 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1">
-        <v>42705</v>
+        <v>42521</v>
       </c>
       <c r="B2">
-        <v>0.7544169598247999</v>
+        <v>0.6569226555692097</v>
       </c>
       <c r="C2" s="1">
-        <v>42172</v>
+        <v>42163</v>
       </c>
       <c r="D2">
-        <v>0.5294593417374607</v>
+        <v>0.6519596988471016</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1">
-        <v>42670</v>
+        <v>41611</v>
       </c>
       <c r="B3">
-        <v>0.6600846051352968</v>
+        <v>0.7680884822188655</v>
       </c>
       <c r="C3" s="1">
-        <v>42325</v>
+        <v>42316</v>
       </c>
       <c r="D3">
-        <v>0.7418251605958088</v>
+        <v>0.6824774982549895</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
-        <v>43251</v>
+        <v>41590</v>
       </c>
       <c r="B4">
-        <v>0.5695315055726758</v>
+        <v>0.7264072648398998</v>
       </c>
       <c r="C4" s="1">
-        <v>41960</v>
+        <v>41951</v>
       </c>
       <c r="D4">
-        <v>0.7218596528130886</v>
+        <v>0.663453098271259</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1">
-        <v>41634</v>
+        <v>42808</v>
       </c>
       <c r="B5">
-        <v>0.7727947502166728</v>
+        <v>0.646734165342685</v>
       </c>
       <c r="C5" s="1">
-        <v>41595</v>
+        <v>41586</v>
       </c>
       <c r="D5">
-        <v>0.6424684675441303</v>
+        <v>0.6765998667174535</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1">
-        <v>42096</v>
+        <v>42332</v>
       </c>
       <c r="B6">
-        <v>0.6769847688264982</v>
+        <v>0.6824774982549895</v>
       </c>
       <c r="C6" s="1">
-        <v>41899</v>
+        <v>41890</v>
       </c>
       <c r="D6">
-        <v>0.6902728225478132</v>
+        <v>0.6207026132692334</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1">
-        <v>41879</v>
+        <v>41338</v>
       </c>
       <c r="B7">
-        <v>0.722130619179442</v>
+        <v>0.6645881065354257</v>
       </c>
       <c r="C7" s="1">
-        <v>41868</v>
+        <v>41859</v>
       </c>
       <c r="D7">
-        <v>0.722130619179442</v>
+        <v>0.7377846179765103</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1">
-        <v>42089</v>
+        <v>41926</v>
       </c>
       <c r="B8">
-        <v>0.6733545037251498</v>
+        <v>0.7250854334051009</v>
       </c>
       <c r="C8" s="1">
-        <v>41807</v>
+        <v>42102</v>
       </c>
       <c r="D8">
-        <v>0.6881080735495126</v>
+        <v>0.7413448017092269</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1">
-        <v>42061</v>
+        <v>42731</v>
       </c>
       <c r="B9">
-        <v>0.7274355670369012</v>
+        <v>0.6848177962019824</v>
       </c>
       <c r="C9" s="1">
-        <v>42507</v>
+        <v>41798</v>
       </c>
       <c r="D9">
-        <v>0.6971074452403934</v>
+        <v>0.7431724685464136</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1">
-        <v>43181</v>
+        <v>43074</v>
       </c>
       <c r="B10">
-        <v>0.6540516691622977</v>
+        <v>0.6366893565009638</v>
       </c>
       <c r="C10" s="1">
-        <v>41776</v>
+        <v>42498</v>
       </c>
       <c r="D10">
-        <v>0.7736173574090093</v>
+        <v>0.6569226555692097</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1">
-        <v>42257</v>
+        <v>42892</v>
       </c>
       <c r="B11">
-        <v>0.6783696404900025</v>
+        <v>0.6442295977179335</v>
       </c>
       <c r="C11" s="1">
-        <v>42568</v>
+        <v>41616</v>
       </c>
       <c r="D11">
-        <v>0.6219145132996855</v>
+        <v>0.7225469330760531</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
-        <v>43006</v>
+        <v>41723</v>
       </c>
       <c r="B12">
-        <v>0.6528797069815229</v>
+        <v>0.5841087002001577</v>
       </c>
       <c r="C12" s="1">
-        <v>42021</v>
+        <v>42559</v>
       </c>
       <c r="D12">
-        <v>0.5718417786564336</v>
+        <v>0.7356672306171231</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1">
-        <v>42684</v>
+        <v>42437</v>
       </c>
       <c r="B13">
-        <v>0.6988892796668139</v>
+        <v>0.610190901296614</v>
       </c>
       <c r="C13" s="1">
-        <v>42355</v>
+        <v>42012</v>
       </c>
       <c r="D13">
-        <v>0.6822130512208228</v>
+        <v>0.6492791626004607</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
-        <v>42187</v>
+        <v>42157</v>
       </c>
       <c r="B14">
-        <v>0.6136022820125115</v>
+        <v>0.64668174041159</v>
       </c>
       <c r="C14" s="1">
-        <v>42538</v>
+        <v>42346</v>
       </c>
       <c r="D14">
-        <v>0.6637142534442962</v>
+        <v>0.6878651725749189</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1">
-        <v>42460</v>
+        <v>42472</v>
       </c>
       <c r="B15">
-        <v>0.5367451933393307</v>
+        <v>0.7116247495068152</v>
       </c>
       <c r="C15" s="1">
-        <v>43268</v>
+        <v>42529</v>
       </c>
       <c r="D15">
-        <v>0.6419817205821515</v>
+        <v>0.7033015841199878</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1">
-        <v>41788</v>
+        <v>42465</v>
       </c>
       <c r="B16">
-        <v>0.7736173574090093</v>
+        <v>0.7022686570707937</v>
       </c>
       <c r="C16" s="1">
-        <v>43086</v>
+        <v>41433</v>
       </c>
       <c r="D16">
-        <v>0.564103747176483</v>
+        <v>0.5749486033930213</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1">
-        <v>42481</v>
+        <v>42150</v>
       </c>
       <c r="B17">
-        <v>0.6596196567039506</v>
+        <v>0.7427383618847421</v>
       </c>
       <c r="C17" s="1">
-        <v>42599</v>
+        <v>41494</v>
       </c>
       <c r="D17">
-        <v>0.6629967999551547</v>
+        <v>0.7473045905800282</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1">
-        <v>41697</v>
+        <v>42612</v>
       </c>
       <c r="B18">
-        <v>0.6856616094172349</v>
+        <v>0.6240145013768331</v>
       </c>
       <c r="C18" s="1">
-        <v>41837</v>
+        <v>41463</v>
       </c>
       <c r="D18">
-        <v>0.7021746615673217</v>
+        <v>0.7069066671692239</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1">
-        <v>41872</v>
+        <v>42276</v>
       </c>
       <c r="B19">
-        <v>0.7899586328646955</v>
+        <v>0.6345610545340595</v>
       </c>
       <c r="C19" s="1">
-        <v>41564</v>
+        <v>41525</v>
       </c>
       <c r="D19">
-        <v>0.6736685883006335</v>
+        <v>0.619885290708389</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1">
-        <v>42243</v>
+        <v>41821</v>
       </c>
       <c r="B20">
-        <v>0.6731717308871218</v>
+        <v>0.6515929453050627</v>
       </c>
       <c r="C20" s="1">
-        <v>43117</v>
+        <v>41828</v>
       </c>
       <c r="D20">
-        <v>0.6354309469450905</v>
+        <v>0.7056208474358152</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1">
-        <v>41732</v>
+        <v>42997</v>
       </c>
       <c r="B21">
-        <v>0.5937713403714721</v>
+        <v>0.5755799679772153</v>
       </c>
       <c r="C21" s="1">
-        <v>42202</v>
+        <v>41555</v>
       </c>
       <c r="D21">
-        <v>0.6994783967580136</v>
+        <v>0.5891765793796149</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1">
-        <v>42537</v>
+        <v>42661</v>
       </c>
       <c r="B22">
-        <v>0.6952750141220236</v>
+        <v>0.629422570316978</v>
       </c>
       <c r="C22" s="1">
-        <v>42783</v>
+        <v>41767</v>
       </c>
       <c r="D22">
-        <v>0.5500941448141663</v>
+        <v>0.7068916740064726</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1">
-        <v>42803</v>
+        <v>42738</v>
       </c>
       <c r="B23">
-        <v>0.6354732363386342</v>
+        <v>0.7330188444884792</v>
       </c>
       <c r="C23" s="1">
-        <v>41746</v>
+        <v>41282</v>
       </c>
       <c r="D23">
-        <v>0.7089609595512552</v>
+        <v>0.6956168992557527</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1">
-        <v>41627</v>
+        <v>42136</v>
       </c>
       <c r="B24">
-        <v>0.5933361822311537</v>
+        <v>0.6691014037218436</v>
       </c>
       <c r="C24" s="1">
-        <v>42052</v>
+        <v>42774</v>
       </c>
       <c r="D24">
-        <v>0.7274355670369012</v>
+        <v>0.6650388543163518</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1">
-        <v>42530</v>
+        <v>41870</v>
       </c>
       <c r="B25">
-        <v>0.7081849908650758</v>
+        <v>0.5864284889564217</v>
       </c>
       <c r="C25" s="1">
-        <v>41687</v>
+        <v>41737</v>
       </c>
       <c r="D25">
-        <v>0.6856616094172349</v>
+        <v>0.7637775558954696</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1">
-        <v>42824</v>
+        <v>41282</v>
       </c>
       <c r="B26">
-        <v>0.6990473136134771</v>
+        <v>0.7340080269854634</v>
       </c>
       <c r="C26" s="1">
-        <v>42630</v>
+        <v>42071</v>
       </c>
       <c r="D26">
-        <v>0.6612001052857946</v>
+        <v>0.7302017768937603</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1">
-        <v>42348</v>
+        <v>42381</v>
       </c>
       <c r="B27">
-        <v>0.6239767582119179</v>
+        <v>0.6896518891436907</v>
       </c>
       <c r="C27" s="1">
-        <v>42080</v>
+        <v>41372</v>
       </c>
       <c r="D27">
-        <v>0.6733545037251498</v>
+        <v>0.6604973124685967</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1">
-        <v>41669</v>
+        <v>42038</v>
       </c>
       <c r="B28">
-        <v>0.6139803496781654</v>
+        <v>0.6478845716120842</v>
       </c>
       <c r="C28" s="1">
-        <v>42691</v>
+        <v>41678</v>
       </c>
       <c r="D28">
-        <v>0.6012430231004323</v>
+        <v>0.6984410128692715</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1">
-        <v>42677</v>
+        <v>41401</v>
       </c>
       <c r="B29">
-        <v>0.7482230836335387</v>
+        <v>0.673023802417635</v>
       </c>
       <c r="C29" s="1">
-        <v>42141</v>
+        <v>42621</v>
       </c>
       <c r="D29">
-        <v>0.68160900779394</v>
+        <v>0.7072051698493358</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1">
-        <v>42740</v>
+        <v>41513</v>
       </c>
       <c r="B30">
-        <v>0.7257031787163855</v>
+        <v>0.7473045905800282</v>
       </c>
       <c r="C30" s="1">
-        <v>42811</v>
+        <v>42743</v>
       </c>
       <c r="D30">
-        <v>0.6990473136134771</v>
+        <v>0.546309531996694</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1">
-        <v>43090</v>
+        <v>41555</v>
       </c>
       <c r="B31">
-        <v>0.6875450545120431</v>
+        <v>0.6943565974034311</v>
       </c>
       <c r="C31" s="1">
-        <v>42660</v>
+        <v>42682</v>
       </c>
       <c r="D31">
-        <v>0.6600846051352968</v>
+        <v>0.7290775089161624</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1">
-        <v>41949</v>
+        <v>41800</v>
       </c>
       <c r="B32">
-        <v>0.7113775534996255</v>
+        <v>0.687809336606237</v>
       </c>
       <c r="C32" s="1">
-        <v>42417</v>
+        <v>41341</v>
       </c>
       <c r="D32">
-        <v>0.6574009385611868</v>
+        <v>0.6631109084624741</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1">
-        <v>41809</v>
+        <v>41625</v>
       </c>
       <c r="B33">
-        <v>0.7241726608473598</v>
+        <v>0.6187404361004675</v>
       </c>
       <c r="C33" s="1">
-        <v>42721</v>
+        <v>42802</v>
       </c>
       <c r="D33">
-        <v>0.5744620352415269</v>
+        <v>0.6091767735424645</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1">
-        <v>42453</v>
+        <v>41968</v>
       </c>
       <c r="B34">
-        <v>0.5302494576122307</v>
+        <v>0.663453098271259</v>
       </c>
       <c r="C34" s="1">
-        <v>41715</v>
+        <v>42651</v>
       </c>
       <c r="D34">
-        <v>0.4401581407126131</v>
+        <v>0.7756178290353026</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1">
-        <v>41781</v>
+        <v>41688</v>
       </c>
       <c r="B35">
-        <v>0.7147331049349273</v>
+        <v>0.6305400028636154</v>
       </c>
       <c r="C35" s="1">
-        <v>43390</v>
+        <v>42043</v>
       </c>
       <c r="D35">
-        <v>0.6645414500039726</v>
+        <v>0.6698187646372949</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1">
-        <v>42488</v>
+        <v>41772</v>
       </c>
       <c r="B36">
-        <v>0.6205818320553416</v>
+        <v>0.6967301597784866</v>
       </c>
       <c r="C36" s="1">
-        <v>43298</v>
+        <v>42712</v>
       </c>
       <c r="D36">
-        <v>0.6742388037090337</v>
+        <v>0.6848177962019824</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1">
-        <v>42628</v>
+        <v>42717</v>
       </c>
       <c r="B37">
-        <v>0.6693579373228765</v>
+        <v>0.7369706789607274</v>
       </c>
       <c r="C37" s="1">
-        <v>42233</v>
+        <v>41706</v>
       </c>
       <c r="D37">
-        <v>0.6731717308871218</v>
+        <v>0.5841087002001577</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1">
-        <v>43279</v>
+        <v>41681</v>
       </c>
       <c r="B38">
-        <v>0.6419817205821515</v>
+        <v>0.6733730939088683</v>
       </c>
       <c r="C38" s="1">
-        <v>41656</v>
+        <v>43077</v>
       </c>
       <c r="D38">
-        <v>0.6139803496781654</v>
+        <v>0.7730262840857649</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1">
-        <v>41921</v>
+        <v>42941</v>
       </c>
       <c r="B39">
-        <v>0.7147527072015264</v>
+        <v>0.6232579626894371</v>
       </c>
       <c r="C39" s="1">
-        <v>42264</v>
+        <v>42224</v>
       </c>
       <c r="D39">
-        <v>0.6289543740659138</v>
+        <v>0.6180283071262735</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1">
-        <v>41837</v>
+        <v>41457</v>
       </c>
       <c r="B40">
-        <v>0.686994239776626</v>
+        <v>0.7263507756728165</v>
       </c>
       <c r="C40" s="1">
-        <v>42111</v>
+        <v>41647</v>
       </c>
       <c r="D40">
-        <v>0.7180366367121926</v>
+        <v>0.7450433194150691</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1">
-        <v>42544</v>
+        <v>42227</v>
       </c>
       <c r="B41">
-        <v>0.6613459734839271</v>
+        <v>0.6146442784872405</v>
       </c>
       <c r="C41" s="1">
-        <v>43207</v>
+        <v>42590</v>
       </c>
       <c r="D41">
-        <v>0.6490691281986285</v>
+        <v>0.6240145013768331</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1">
-        <v>41620</v>
+        <v>41478</v>
       </c>
       <c r="B42">
-        <v>0.6043937536765693</v>
+        <v>0.6214625888388735</v>
       </c>
       <c r="C42" s="1">
-        <v>42752</v>
+        <v>41313</v>
       </c>
       <c r="D42">
-        <v>0.7256803769509129</v>
+        <v>0.7684770458014135</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1">
-        <v>42110</v>
+        <v>41296</v>
       </c>
       <c r="B43">
-        <v>0.7233872453455421</v>
+        <v>0.7463204122493914</v>
       </c>
       <c r="C43" s="1">
-        <v>42842</v>
+        <v>41402</v>
       </c>
       <c r="D43">
-        <v>0.6043800914014212</v>
+        <v>0.6229403963118411</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1">
-        <v>42145</v>
+        <v>42143</v>
       </c>
       <c r="B44">
-        <v>0.7961833958195174</v>
+        <v>0.6748136271462712</v>
       </c>
       <c r="C44" s="1">
-        <v>42872</v>
+        <v>42833</v>
       </c>
       <c r="D44">
-        <v>0.6552470204050731</v>
+        <v>0.6173698011057647</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1">
-        <v>42642</v>
+        <v>41289</v>
       </c>
       <c r="B45">
-        <v>0.6612001052857946</v>
+        <v>0.6225703845096703</v>
       </c>
       <c r="C45" s="1">
-        <v>41625</v>
+        <v>42193</v>
       </c>
       <c r="D45">
-        <v>0.7727947502166728</v>
+        <v>0.6024332770651848</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="1">
-        <v>42831</v>
+        <v>42374</v>
       </c>
       <c r="B46">
-        <v>0.5681121866880915</v>
+        <v>0.6806787411698385</v>
       </c>
       <c r="C46" s="1">
-        <v>43056</v>
+        <v>42132</v>
       </c>
       <c r="D46">
-        <v>0.5627523214339655</v>
+        <v>0.7427383618847421</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="1">
-        <v>42397</v>
+        <v>42080</v>
       </c>
       <c r="B47">
-        <v>0.653862895309344</v>
+        <v>0.7313859274443433</v>
       </c>
       <c r="C47" s="1">
-        <v>43360</v>
+        <v>43047</v>
       </c>
       <c r="D47">
-        <v>0.6328592896306919</v>
+        <v>0.595922212135094</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="1">
-        <v>42047</v>
+        <v>41408</v>
       </c>
       <c r="B48">
-        <v>0.7209406677905889</v>
+        <v>0.7323665879059381</v>
       </c>
       <c r="C48" s="1">
-        <v>42995</v>
+        <v>42863</v>
       </c>
       <c r="D48">
-        <v>0.6528797069815229</v>
+        <v>0.6372801911851695</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="1">
-        <v>42054</v>
+        <v>42416</v>
       </c>
       <c r="B49">
-        <v>0.7335419722358061</v>
+        <v>0.7244716309418211</v>
       </c>
       <c r="C49" s="1">
-        <v>41990</v>
+        <v>42986</v>
       </c>
       <c r="D49">
-        <v>0.7140442163425779</v>
+        <v>0.7028247521497526</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1">
-        <v>42033</v>
+        <v>42906</v>
       </c>
       <c r="B50">
-        <v>0.5718417786564336</v>
+        <v>0.5920170174777987</v>
       </c>
       <c r="C50" s="1">
-        <v>43237</v>
+        <v>41981</v>
       </c>
       <c r="D50">
-        <v>0.5695315055726758</v>
+        <v>0.517423470738716</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="1">
-        <v>42201</v>
+        <v>41653</v>
       </c>
       <c r="B51">
-        <v>0.7066218267623453</v>
+        <v>0.7060205642293195</v>
       </c>
       <c r="C51" s="1">
-        <v>41929</v>
+        <v>42255</v>
       </c>
       <c r="D51">
-        <v>0.712558180797827</v>
+        <v>0.6345610545340595</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="1">
-        <v>41571</v>
+        <v>42430</v>
       </c>
       <c r="B52">
-        <v>0.6565508644578548</v>
+        <v>0.6231824449529941</v>
       </c>
       <c r="C52" s="1">
-        <v>42386</v>
+        <v>42894</v>
       </c>
       <c r="D52">
-        <v>0.653862895309344</v>
+        <v>0.6313261369886903</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="1">
-        <v>42586</v>
+        <v>41450</v>
       </c>
       <c r="B53">
-        <v>0.6852078352874988</v>
+        <v>0.5749486033930213</v>
       </c>
       <c r="C53" s="1">
-        <v>43176</v>
+        <v>41920</v>
       </c>
       <c r="D53">
-        <v>0.7001614537900318</v>
+        <v>0.7137628578088221</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="1">
-        <v>41816</v>
+        <v>41996</v>
       </c>
       <c r="B54">
-        <v>0.6881080735495126</v>
+        <v>0.7258905669821053</v>
       </c>
       <c r="C54" s="1">
-        <v>43148</v>
+        <v>42377</v>
       </c>
       <c r="D54">
-        <v>0.5510745600589146</v>
+        <v>0.6268923440935282</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="1">
-        <v>42194</v>
+        <v>41765</v>
       </c>
       <c r="B55">
-        <v>0.6972809083922765</v>
+        <v>0.7487421024125256</v>
       </c>
       <c r="C55" s="1">
-        <v>42294</v>
+        <v>42285</v>
       </c>
       <c r="D55">
-        <v>0.8294428715812254</v>
+        <v>0.7066547300127269</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="1">
-        <v>43055</v>
+        <v>41835</v>
       </c>
       <c r="B56">
-        <v>0.625622335027436</v>
+        <v>0.7530800816384442</v>
       </c>
       <c r="C56" s="1">
-        <v>42446</v>
+        <v>42437</v>
       </c>
       <c r="D56">
-        <v>0.5367451933393307</v>
+        <v>0.6054397188875477</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="1">
-        <v>42292</v>
+        <v>41506</v>
       </c>
       <c r="B57">
-        <v>0.6775194151697268</v>
+        <v>0.7065176800279668</v>
       </c>
       <c r="C57" s="1">
-        <v>43329</v>
+        <v>43016</v>
       </c>
       <c r="D57">
-        <v>0.5641766911625608</v>
+        <v>0.67681990159216</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="1">
-        <v>42166</v>
+        <v>41660</v>
       </c>
       <c r="B58">
-        <v>0.6038020096216468</v>
+        <v>0.7579177192377183</v>
       </c>
       <c r="C58" s="1">
-        <v>43025</v>
+        <v>42408</v>
       </c>
       <c r="D58">
-        <v>0.6660725800532608</v>
+        <v>0.7324151241088976</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="1">
-        <v>42467</v>
+        <v>43004</v>
       </c>
       <c r="B59">
-        <v>0.7209800305996572</v>
+        <v>0.7028247521497526</v>
       </c>
       <c r="C59" s="1">
-        <v>42903</v>
+        <v>42924</v>
       </c>
       <c r="D59">
-        <v>0.5975913263152937</v>
+        <v>0.6232579626894371</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="1">
-        <v>43293</v>
+        <v>41912</v>
       </c>
       <c r="B60">
-        <v>0.6184318287758273</v>
+        <v>0.6207026132692334</v>
       </c>
       <c r="C60" s="1">
-        <v>42933</v>
+        <v>42955</v>
       </c>
       <c r="D60">
-        <v>0.6552916719241484</v>
+        <v>0.5015741537649527</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="1">
-        <v>42215</v>
+        <v>42528</v>
       </c>
       <c r="B61">
-        <v>0.6994783967580136</v>
+        <v>0.7118408067672931</v>
       </c>
       <c r="C61" s="1">
-        <v>42964</v>
+        <v>42468</v>
       </c>
       <c r="D61">
-        <v>0.5583653891676852</v>
+        <v>0.606392610525103</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="1">
-        <v>41746</v>
+        <v>41877</v>
       </c>
       <c r="B62">
-        <v>0.6721467309918663</v>
-      </c>
-      <c r="C62" s="1">
-        <v>42477</v>
-      </c>
-      <c r="D62">
-        <v>0.6205818320553416</v>
+        <v>0.7377846179765103</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="1">
-        <v>41928</v>
+        <v>42087</v>
       </c>
       <c r="B63">
-        <v>0.6896428867532366</v>
+        <v>0.6243808103152481</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="1">
-        <v>42733</v>
+        <v>41793</v>
       </c>
       <c r="B64">
-        <v>0.5744620352415269</v>
+        <v>0.6105324220669548</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="1">
-        <v>41739</v>
+        <v>41345</v>
       </c>
       <c r="B65">
-        <v>0.5786080769644668</v>
+        <v>0.7092350127954749</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="1">
-        <v>41613</v>
+        <v>42024</v>
       </c>
       <c r="B66">
-        <v>0.5734595340449505</v>
+        <v>0.6648176875592422</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="1">
-        <v>42159</v>
+        <v>41548</v>
       </c>
       <c r="B67">
-        <v>0.7053843441898326</v>
+        <v>0.6138890348850267</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="1">
-        <v>42313</v>
+        <v>41394</v>
       </c>
       <c r="B68">
-        <v>0.6861461268522532</v>
+        <v>0.6604973124685967</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="1">
-        <v>42152</v>
+        <v>41520</v>
       </c>
       <c r="B69">
-        <v>0.68160900779394</v>
+        <v>0.7715166116978935</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="1">
-        <v>41704</v>
+        <v>42962</v>
       </c>
       <c r="B70">
-        <v>0.6831760955657386</v>
+        <v>0.7162205524363888</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="1">
-        <v>43020</v>
+        <v>42794</v>
       </c>
       <c r="B71">
-        <v>0.7156831835622839</v>
+        <v>0.6650388543163518</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="1">
-        <v>42698</v>
+        <v>42927</v>
       </c>
       <c r="B72">
-        <v>0.6012430231004323</v>
+        <v>0.5290470486645781</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="1">
-        <v>42390</v>
+        <v>42724</v>
       </c>
       <c r="B73">
-        <v>0.6100489498048478</v>
+        <v>0.5750012018524568</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="1">
-        <v>42341</v>
+        <v>42423</v>
       </c>
       <c r="B74">
-        <v>0.729708555146042</v>
+        <v>0.7324151241088976</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="1">
-        <v>42418</v>
+        <v>42241</v>
       </c>
       <c r="B75">
-        <v>0.7142416328103292</v>
+        <v>0.6180283071262735</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="1">
-        <v>42880</v>
+        <v>41730</v>
       </c>
       <c r="B76">
-        <v>0.6552470204050731</v>
+        <v>0.7860896178740854</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="1">
-        <v>42208</v>
+        <v>41464</v>
       </c>
       <c r="B77">
-        <v>0.7029285080081725</v>
+        <v>0.6834987590649034</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="1">
-        <v>43076</v>
+        <v>41905</v>
       </c>
       <c r="B78">
-        <v>0.5695681121933052</v>
+        <v>0.6706346246127087</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="1">
-        <v>41795</v>
+        <v>42773</v>
       </c>
       <c r="B79">
-        <v>0.6169445549851986</v>
+        <v>0.5675309142379793</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="1">
-        <v>42495</v>
+        <v>41443</v>
       </c>
       <c r="B80">
-        <v>0.714340398765565</v>
+        <v>0.6900645572169728</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="1">
-        <v>42439</v>
+        <v>41485</v>
       </c>
       <c r="B81">
-        <v>0.6592988680105857</v>
+        <v>0.7069066671692239</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="1">
-        <v>43237</v>
+        <v>41303</v>
       </c>
       <c r="B82">
-        <v>0.6490967698751677</v>
+        <v>0.6956168992557527</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="1">
-        <v>42005</v>
+        <v>41597</v>
       </c>
       <c r="B83">
-        <v>0.599213410649613</v>
+        <v>0.6878116685315913</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="1">
-        <v>43370</v>
+        <v>41352</v>
       </c>
       <c r="B84">
-        <v>0.6328592896306919</v>
+        <v>0.7297677232219052</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="1">
-        <v>42446</v>
+        <v>42346</v>
       </c>
       <c r="B85">
-        <v>0.7433324323114667</v>
+        <v>0.7609557725867632</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="1">
-        <v>42901</v>
+        <v>42850</v>
       </c>
       <c r="B86">
-        <v>0.6761048532591891</v>
+        <v>0.6173698011057647</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="1">
-        <v>41851</v>
+        <v>42577</v>
       </c>
       <c r="B87">
-        <v>0.7021746615673217</v>
+        <v>0.7356672306171231</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="1">
-        <v>43258</v>
+        <v>41646</v>
       </c>
       <c r="B88">
-        <v>0.4929316334981884</v>
+        <v>0.5671266030429896</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="1">
-        <v>42516</v>
+        <v>41527</v>
       </c>
       <c r="B89">
-        <v>0.6971074452403934</v>
+        <v>0.7088834495661555</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="1">
-        <v>43188</v>
+        <v>42192</v>
       </c>
       <c r="B90">
-        <v>0.7001614537900318</v>
+        <v>0.6533151525822221</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="1">
-        <v>42551</v>
+        <v>42304</v>
       </c>
       <c r="B91">
-        <v>0.6637142534442962</v>
+        <v>0.7066547300127269</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="1">
-        <v>41977</v>
+        <v>41947</v>
       </c>
       <c r="B92">
-        <v>0.6752057262429408</v>
+        <v>0.6733086005753232</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="1">
-        <v>42131</v>
+        <v>42955</v>
       </c>
       <c r="B93">
-        <v>0.6832154060065078</v>
+        <v>0.5916881617919814</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="1">
-        <v>43307</v>
+        <v>42787</v>
       </c>
       <c r="B94">
-        <v>0.6742388037090337</v>
+        <v>0.6554428732172</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="1">
-        <v>41690</v>
+        <v>42094</v>
       </c>
       <c r="B95">
-        <v>0.7472297190191682</v>
+        <v>0.7302017768937603</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="1">
-        <v>42502</v>
+        <v>41492</v>
       </c>
       <c r="B96">
-        <v>0.620662903495947</v>
+        <v>0.6323202093989559</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="1">
-        <v>43118</v>
+        <v>42262</v>
       </c>
       <c r="B97">
-        <v>0.5898240010803975</v>
+        <v>0.6839893291761672</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="1">
-        <v>42040</v>
+        <v>42745</v>
       </c>
       <c r="B98">
-        <v>0.7288826331922816</v>
+        <v>0.6085203799204407</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="1">
-        <v>41683</v>
+        <v>41429</v>
       </c>
       <c r="B99">
-        <v>0.8046082806442801</v>
+        <v>0.6933255228469642</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="1">
-        <v>42019</v>
+        <v>42500</v>
       </c>
       <c r="B100">
-        <v>0.6505403813415211</v>
+        <v>0.6573368812809571</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="1">
-        <v>42915</v>
+        <v>41975</v>
       </c>
       <c r="B101">
-        <v>0.5975913263152937</v>
+        <v>0.6887245124055543</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="1">
-        <v>41802</v>
+        <v>42535</v>
       </c>
       <c r="B102">
-        <v>0.7059694892897188</v>
+        <v>0.6808856959328985</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="1">
-        <v>41984</v>
+        <v>41989</v>
       </c>
       <c r="B103">
-        <v>0.7349130704330761</v>
+        <v>0.7564938291552981</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="1">
-        <v>41564</v>
+        <v>42640</v>
       </c>
       <c r="B104">
-        <v>0.6681880957501631</v>
+        <v>0.7072051698493358</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="1">
-        <v>42383</v>
+        <v>42843</v>
       </c>
       <c r="B105">
-        <v>0.6729752444586077</v>
+        <v>0.6692488494150616</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="1">
-        <v>42558</v>
+        <v>41674</v>
       </c>
       <c r="B106">
-        <v>0.6564073129854081</v>
+        <v>0.6814615735450862</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="1">
-        <v>43321</v>
+        <v>42969</v>
       </c>
       <c r="B107">
-        <v>0.5884578375612289</v>
+        <v>0.661200875639313</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="1">
-        <v>42236</v>
+        <v>42010</v>
       </c>
       <c r="B108">
-        <v>0.6227451627175554</v>
+        <v>0.6338153950263519</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="1">
-        <v>43286</v>
+        <v>42045</v>
       </c>
       <c r="B109">
-        <v>0.5285554846522963</v>
+        <v>0.7054182173696283</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="1">
-        <v>42719</v>
+        <v>41499</v>
       </c>
       <c r="B110">
-        <v>0.6683230367827924</v>
+        <v>0.6725421519016103</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="1">
-        <v>42607</v>
+        <v>41898</v>
       </c>
       <c r="B111">
-        <v>0.6629967999551547</v>
+        <v>0.688024568127471</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="1">
-        <v>41753</v>
+        <v>41387</v>
       </c>
       <c r="B112">
-        <v>0.7089609595512552</v>
+        <v>0.7042890565911577</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="1">
-        <v>42943</v>
+        <v>42185</v>
       </c>
       <c r="B113">
-        <v>0.6552916719241484</v>
+        <v>0.6519596988471016</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" s="1">
-        <v>42509</v>
+        <v>41583</v>
       </c>
       <c r="B114">
-        <v>0.6644614292358818</v>
+        <v>0.6851835975627423</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="1">
-        <v>41655</v>
+        <v>42948</v>
       </c>
       <c r="B115">
-        <v>0.6889674504103879</v>
+        <v>0.6638072839110211</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="1">
-        <v>42754</v>
+        <v>42129</v>
       </c>
       <c r="B116">
-        <v>0.7369607925121174</v>
+        <v>0.7493508672962341</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="1">
-        <v>42138</v>
+        <v>42710</v>
       </c>
       <c r="B117">
-        <v>0.7243863977328693</v>
+        <v>0.6403802459423809</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="1">
-        <v>41718</v>
+        <v>42269</v>
       </c>
       <c r="B118">
-        <v>0.6930261944702292</v>
+        <v>0.707590719280362</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="1">
-        <v>42768</v>
+        <v>41562</v>
       </c>
       <c r="B119">
-        <v>0.6762623229566205</v>
+        <v>0.6810615699709726</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="1">
-        <v>42320</v>
+        <v>42591</v>
       </c>
       <c r="B120">
-        <v>0.6631547933832603</v>
+        <v>0.5734754009601122</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="1">
-        <v>42747</v>
+        <v>41737</v>
       </c>
       <c r="B121">
-        <v>0.583084628892933</v>
+        <v>0.7259173583543448</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" s="1">
-        <v>42873</v>
+        <v>42493</v>
       </c>
       <c r="B122">
-        <v>0.6146429998558783</v>
+        <v>0.5224887619150801</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" s="1">
-        <v>42250</v>
+        <v>41569</v>
       </c>
       <c r="B123">
-        <v>0.7497719462616023</v>
+        <v>0.7934311598302964</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="1">
-        <v>42103</v>
+        <v>43088</v>
       </c>
       <c r="B124">
-        <v>0.6938800842549995</v>
+        <v>0.6426179032155469</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="1">
-        <v>41900</v>
+        <v>42703</v>
       </c>
       <c r="B125">
-        <v>0.7364707432486849</v>
+        <v>0.7290775089161624</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="1">
-        <v>42362</v>
+        <v>41842</v>
       </c>
       <c r="B126">
-        <v>0.6971804647490593</v>
+        <v>0.6028059098473737</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="1">
-        <v>41991</v>
+        <v>41702</v>
       </c>
       <c r="B127">
-        <v>0.7134867858190258</v>
+        <v>0.6539930789463327</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="1">
-        <v>42229</v>
+        <v>43018</v>
       </c>
       <c r="B128">
-        <v>0.6053386914575332</v>
+        <v>0.6074871868866881</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="1">
-        <v>41858</v>
+        <v>41604</v>
       </c>
       <c r="B129">
-        <v>0.7378295087066888</v>
+        <v>0.6765998667174535</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="1">
-        <v>42432</v>
+        <v>42857</v>
       </c>
       <c r="B130">
-        <v>0.5551404917433894</v>
+        <v>0.6910867504062002</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" s="1">
-        <v>41963</v>
+        <v>42339</v>
       </c>
       <c r="B131">
-        <v>0.7726171521233625</v>
+        <v>0.7271307131225244</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="1">
-        <v>42124</v>
+        <v>41373</v>
       </c>
       <c r="B132">
-        <v>0.7180366367121926</v>
+        <v>0.7098033918605491</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="1">
-        <v>42971</v>
+        <v>42605</v>
       </c>
       <c r="B133">
-        <v>0.5461086686043629</v>
+        <v>0.7027854418314147</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" s="1">
-        <v>42796</v>
+        <v>41422</v>
       </c>
       <c r="B134">
-        <v>0.6508848672114061</v>
+        <v>0.6229403963118411</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" s="1">
-        <v>42985</v>
+        <v>42206</v>
       </c>
       <c r="B135">
-        <v>0.6402345306021237</v>
+        <v>0.6764348182629096</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="1">
-        <v>42649</v>
+        <v>41891</v>
       </c>
       <c r="B136">
-        <v>0.5829353789243802</v>
+        <v>0.7384708639028787</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" s="1">
-        <v>42579</v>
+        <v>41380</v>
       </c>
       <c r="B137">
-        <v>0.6219145132996855</v>
+        <v>0.6842271796531986</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="1">
-        <v>43265</v>
+        <v>42178</v>
       </c>
       <c r="B138">
-        <v>0.6798671066408298</v>
+        <v>0.6871193927441076</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" s="1">
-        <v>42761</v>
+        <v>42199</v>
       </c>
       <c r="B139">
-        <v>0.7256803769509129</v>
+        <v>0.7534277898412942</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="1">
-        <v>41774</v>
+        <v>43053</v>
       </c>
       <c r="B140">
-        <v>0.6165927627645127</v>
+        <v>0.6169791462538046</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="1">
-        <v>43132</v>
+        <v>42108</v>
       </c>
       <c r="B141">
-        <v>0.6092516510104984</v>
+        <v>0.7317975244002785</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="1">
-        <v>41760</v>
+        <v>41471</v>
       </c>
       <c r="B142">
-        <v>0.6510704847520746</v>
+        <v>0.6725365109703825</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="1">
-        <v>43300</v>
+        <v>41933</v>
       </c>
       <c r="B143">
-        <v>0.7215917501720737</v>
+        <v>0.7618474706616517</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="1">
-        <v>43153</v>
+        <v>41849</v>
       </c>
       <c r="B144">
-        <v>0.5510745600589146</v>
+        <v>0.7056208474358152</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" s="1">
-        <v>43377</v>
+        <v>41317</v>
       </c>
       <c r="B145">
-        <v>0.6645414500039726</v>
+        <v>0.7720758009498878</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" s="1">
-        <v>42929</v>
+        <v>42598</v>
       </c>
       <c r="B146">
-        <v>0.6254983914094957</v>
+        <v>0.658251733338765</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" s="1">
-        <v>42026</v>
+        <v>42668</v>
       </c>
       <c r="B147">
-        <v>0.7046801849856138</v>
+        <v>0.7756178290353026</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="1">
-        <v>41998</v>
+        <v>42934</v>
       </c>
       <c r="B148">
-        <v>0.7140442163425779</v>
+        <v>0.5750813024355192</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="1">
-        <v>42222</v>
+        <v>42514</v>
       </c>
       <c r="B149">
-        <v>0.6810480728517224</v>
+        <v>0.5431277962320327</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" s="1">
-        <v>42425</v>
+        <v>42549</v>
       </c>
       <c r="B150">
-        <v>0.6574009385611868</v>
+        <v>0.7033015841199878</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" s="1">
-        <v>41606</v>
+        <v>42696</v>
       </c>
       <c r="B151">
-        <v>0.6424684675441303</v>
+        <v>0.7016615277929562</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="1">
-        <v>41956</v>
+        <v>41415</v>
       </c>
       <c r="B152">
-        <v>0.7137485030697713</v>
+        <v>0.7203876512845039</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" s="1">
-        <v>42117</v>
+        <v>43060</v>
       </c>
       <c r="B153">
-        <v>0.7863271699514558</v>
+        <v>0.5983365478508224</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" s="1">
-        <v>41599</v>
+        <v>42444</v>
       </c>
       <c r="B154">
-        <v>0.6298796895401165</v>
+        <v>0.6132978417612206</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" s="1">
-        <v>43041</v>
+        <v>42059</v>
       </c>
       <c r="B155">
-        <v>0.5598952563796176</v>
+        <v>0.6698187646372949</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" s="1">
-        <v>42964</v>
+        <v>42913</v>
       </c>
       <c r="B156">
-        <v>0.7090862007962205</v>
+        <v>0.6313261369886903</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" s="1">
-        <v>43272</v>
+        <v>42542</v>
       </c>
       <c r="B157">
-        <v>0.5550236072329617</v>
+        <v>0.5665402957029781</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" s="1">
-        <v>42264</v>
+        <v>41751</v>
       </c>
       <c r="B158">
-        <v>0.7262376890981445</v>
+        <v>0.7191564305508016</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" s="1">
-        <v>42726</v>
+        <v>42290</v>
       </c>
       <c r="B159">
-        <v>0.6350624231993589</v>
+        <v>0.721271110617092</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" s="1">
-        <v>41914</v>
+        <v>41884</v>
       </c>
       <c r="B160">
-        <v>0.6875194046088864</v>
+        <v>0.723870473806233</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" s="1">
-        <v>41578</v>
+        <v>41744</v>
       </c>
       <c r="B161">
-        <v>0.6736685883006335</v>
+        <v>0.6694257341648365</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" s="1">
-        <v>43139</v>
+        <v>41982</v>
       </c>
       <c r="B162">
-        <v>0.485024182806808</v>
+        <v>0.6830526679799658</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" s="1">
-        <v>43335</v>
+        <v>41716</v>
       </c>
       <c r="B163">
-        <v>0.577937136989526</v>
+        <v>0.6987449557389719</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" s="1">
-        <v>41711</v>
+        <v>41534</v>
       </c>
       <c r="B164">
-        <v>0.6497961077754307</v>
+        <v>0.5784506231178849</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" s="1">
-        <v>43027</v>
+        <v>42318</v>
       </c>
       <c r="B165">
-        <v>0.6390229020455414</v>
+        <v>0.7080365372443765</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="1">
-        <v>42068</v>
+        <v>42815</v>
       </c>
       <c r="B166">
-        <v>0.6807789647628716</v>
+        <v>0.6488692201828824</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" s="1">
-        <v>41830</v>
+        <v>41639</v>
       </c>
       <c r="B167">
-        <v>0.7388289134995246</v>
+        <v>0.7225469330760531</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" s="1">
-        <v>42852</v>
+        <v>42101</v>
       </c>
       <c r="B168">
-        <v>0.6043800914014212</v>
+        <v>0.6402427361594145</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" s="1">
-        <v>43195</v>
+        <v>41940</v>
       </c>
       <c r="B169">
-        <v>0.5978395494045543</v>
+        <v>0.7137628578088221</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" s="1">
-        <v>42355</v>
+        <v>41310</v>
       </c>
       <c r="B170">
-        <v>0.6973370942220515</v>
+        <v>0.597054629739918</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" s="1">
-        <v>43167</v>
+        <v>42563</v>
       </c>
       <c r="B171">
-        <v>0.7065577630864915</v>
+        <v>0.6617265553523352</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" s="1">
-        <v>43146</v>
+        <v>42507</v>
       </c>
       <c r="B172">
-        <v>0.5135842835904716</v>
+        <v>0.6108500149049063</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" s="1">
-        <v>41907</v>
+        <v>42171</v>
       </c>
       <c r="B173">
-        <v>0.6902728225478132</v>
+        <v>0.6852009614863381</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" s="1">
-        <v>42810</v>
+        <v>42689</v>
       </c>
       <c r="B174">
-        <v>0.6728622983369519</v>
+        <v>0.6598358164174375</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" s="1">
-        <v>41865</v>
+        <v>42752</v>
       </c>
       <c r="B175">
-        <v>0.6458137769479708</v>
+        <v>0.6514962568997551</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" s="1">
-        <v>43223</v>
+        <v>43067</v>
       </c>
       <c r="B176">
-        <v>0.645902219037922</v>
+        <v>0.595922212135094</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" s="1">
-        <v>42957</v>
+        <v>41961</v>
       </c>
       <c r="B177">
-        <v>0.6009168564127044</v>
+        <v>0.7183651440474581</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" s="1">
-        <v>43356</v>
+        <v>43032</v>
       </c>
       <c r="B178">
-        <v>0.5933914328833296</v>
+        <v>0.6286694110652682</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" s="1">
-        <v>42845</v>
+        <v>42871</v>
       </c>
       <c r="B179">
-        <v>0.6288771757260306</v>
+        <v>0.5884841155484293</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" s="1">
-        <v>42978</v>
+        <v>43011</v>
       </c>
       <c r="B180">
-        <v>0.5583653891676852</v>
+        <v>0.6676262900292556</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" s="1">
-        <v>42621</v>
+        <v>41331</v>
       </c>
       <c r="B181">
-        <v>0.6328859975103427</v>
+        <v>0.7684770458014135</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" s="1">
-        <v>42572</v>
+        <v>42864</v>
       </c>
       <c r="B182">
-        <v>0.6525768093015395</v>
+        <v>0.7260155793010956</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" s="1">
-        <v>42992</v>
+        <v>42920</v>
       </c>
       <c r="B183">
-        <v>0.568623851297547</v>
+        <v>0.6010214206342096</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" s="1">
-        <v>42656</v>
+        <v>41919</v>
       </c>
       <c r="B184">
-        <v>0.6866150545915588</v>
+        <v>0.7860385837193323</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" s="1">
-        <v>43342</v>
+        <v>42836</v>
       </c>
       <c r="B185">
-        <v>0.5641766911625608</v>
+        <v>0.672218686373063</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" s="1">
-        <v>43034</v>
+        <v>41366</v>
       </c>
       <c r="B186">
-        <v>0.6660725800532608</v>
+        <v>0.7487580319801354</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" s="1">
-        <v>41598</v>
+        <v>42017</v>
       </c>
       <c r="B187">
-        <v>0.5748477443876296</v>
+        <v>0.6513053749284353</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" s="1">
-        <v>42075</v>
+        <v>42213</v>
       </c>
       <c r="B188">
-        <v>0.625616077204089</v>
+        <v>0.6024332770651848</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" s="1">
-        <v>41676</v>
+        <v>43095</v>
       </c>
       <c r="B189">
-        <v>0.6441707735297685</v>
+        <v>0.7730262840857649</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" s="1">
-        <v>42012</v>
+        <v>41541</v>
       </c>
       <c r="B190">
-        <v>0.7622596632483473</v>
+        <v>0.619885290708389</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" s="1">
-        <v>42565</v>
+        <v>41856</v>
       </c>
       <c r="B191">
-        <v>0.6689178491480742</v>
+        <v>0.7102975556986778</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" s="1">
-        <v>43202</v>
+        <v>41632</v>
       </c>
       <c r="B192">
-        <v>0.6632783638729108</v>
+        <v>0.6431853892747922</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" s="1">
-        <v>42859</v>
+        <v>42122</v>
       </c>
       <c r="B193">
-        <v>0.5981505147193216</v>
+        <v>0.7413448017092269</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" s="1">
-        <v>42299</v>
+        <v>42353</v>
       </c>
       <c r="B194">
-        <v>0.6413238554835999</v>
+        <v>0.7209270734837037</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" s="1">
-        <v>41725</v>
+        <v>42829</v>
       </c>
       <c r="B195">
-        <v>0.4401581407126131</v>
+        <v>0.6255061481075639</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" s="1">
-        <v>41585</v>
+        <v>42983</v>
       </c>
       <c r="B196">
-        <v>0.643108078093125</v>
+        <v>0.7443956818136725</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" s="1">
-        <v>42950</v>
+        <v>42556</v>
       </c>
       <c r="B197">
-        <v>0.6270454848335578</v>
+        <v>0.646013823660907</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" s="1">
-        <v>43125</v>
+        <v>42360</v>
       </c>
       <c r="B198">
-        <v>0.6354309469450905</v>
+        <v>0.6210644589221412</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" s="1">
-        <v>42334</v>
+        <v>42647</v>
       </c>
       <c r="B199">
-        <v>0.7418251605958088</v>
+        <v>0.726945642861757</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" s="1">
-        <v>43083</v>
+        <v>42682</v>
       </c>
       <c r="B200">
-        <v>0.6114338655548264</v>
+        <v>0.7220967131078658</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" s="1">
-        <v>43013</v>
+        <v>42759</v>
       </c>
       <c r="B201">
-        <v>0.686919030710652</v>
+        <v>0.6725526642646247</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" s="1">
-        <v>42173</v>
+        <v>41954</v>
       </c>
       <c r="B202">
-        <v>0.714591002751257</v>
+        <v>0.6798193291225685</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" s="1">
-        <v>42593</v>
+        <v>42633</v>
       </c>
       <c r="B203">
-        <v>0.6487878539621491</v>
+        <v>0.5820097586353643</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204" s="1">
-        <v>42327</v>
+        <v>42458</v>
       </c>
       <c r="B204">
-        <v>0.7163841030860484</v>
+        <v>0.6054397188875477</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" s="1">
-        <v>41641</v>
+        <v>42395</v>
       </c>
       <c r="B205">
-        <v>0.7019635971110356</v>
+        <v>0.6268923440935282</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" s="1">
-        <v>41767</v>
+        <v>41786</v>
       </c>
       <c r="B206">
-        <v>0.6148512411532838</v>
+        <v>0.7068916740064726</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" s="1">
-        <v>42866</v>
+        <v>41667</v>
       </c>
       <c r="B207">
-        <v>0.6797652629955252</v>
+        <v>0.7450433194150691</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" s="1">
-        <v>42782</v>
+        <v>41324</v>
       </c>
       <c r="B208">
-        <v>0.6018650105210331</v>
+        <v>0.6129087931302158</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" s="1">
-        <v>43209</v>
+        <v>41695</v>
       </c>
       <c r="B209">
-        <v>0.6909001232514438</v>
+        <v>0.6984410128692715</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210" s="1">
-        <v>41823</v>
+        <v>41359</v>
       </c>
       <c r="B210">
-        <v>0.6747624411336655</v>
+        <v>0.6631109084624741</v>
       </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" s="1">
-        <v>42936</v>
+        <v>42570</v>
       </c>
       <c r="B211">
-        <v>0.6978091285611076</v>
+        <v>0.6122893051531612</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" s="1">
-        <v>43160</v>
+        <v>42626</v>
       </c>
       <c r="B212">
-        <v>0.6312993934516619</v>
+        <v>0.63753467219716</v>
       </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213" s="1">
-        <v>41662</v>
+        <v>42878</v>
       </c>
       <c r="B213">
-        <v>0.6740811654269716</v>
+        <v>0.7945850433676287</v>
       </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214" s="1">
-        <v>43244</v>
+        <v>41758</v>
       </c>
       <c r="B214">
-        <v>0.6529793274661541</v>
+        <v>0.7637775558954696</v>
       </c>
     </row>
     <row r="215" spans="1:2">
       <c r="A215" s="1">
-        <v>42404</v>
+        <v>42220</v>
       </c>
       <c r="B215">
-        <v>0.6958189161070162</v>
+        <v>0.6655487435775009</v>
       </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216" s="1">
-        <v>42635</v>
+        <v>42801</v>
       </c>
       <c r="B216">
-        <v>0.6568286574307758</v>
+        <v>0.7141026449575745</v>
       </c>
     </row>
     <row r="217" spans="1:2">
       <c r="A217" s="1">
-        <v>43349</v>
+        <v>41709</v>
       </c>
       <c r="B217">
-        <v>0.7036849464867158</v>
+        <v>0.7053923164057422</v>
       </c>
     </row>
     <row r="218" spans="1:2">
       <c r="A218" s="1">
-        <v>42614</v>
+        <v>42115</v>
       </c>
       <c r="B218">
-        <v>0.6346924643551735</v>
+        <v>0.7311623904227389</v>
       </c>
     </row>
     <row r="219" spans="1:2">
       <c r="A219" s="1">
-        <v>41935</v>
+        <v>42325</v>
       </c>
       <c r="B219">
-        <v>0.5144268974933625</v>
+        <v>0.6872532037063857</v>
       </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220" s="1">
-        <v>42369</v>
+        <v>42822</v>
       </c>
       <c r="B220">
-        <v>0.6822130512208228</v>
+        <v>0.6091767735424645</v>
       </c>
     </row>
     <row r="221" spans="1:2">
       <c r="A221" s="1">
-        <v>41886</v>
+        <v>42066</v>
       </c>
       <c r="B221">
-        <v>0.6895533837527611</v>
+        <v>0.7551076592094642</v>
       </c>
     </row>
     <row r="222" spans="1:2">
       <c r="A222" s="1">
-        <v>42600</v>
+        <v>42479</v>
       </c>
       <c r="B222">
-        <v>0.6406862300788824</v>
+        <v>0.7827559185215861</v>
       </c>
     </row>
     <row r="223" spans="1:2">
       <c r="A223" s="1">
-        <v>42999</v>
+        <v>42402</v>
       </c>
       <c r="B223">
-        <v>0.5914216023523876</v>
+        <v>0.6578816107637041</v>
       </c>
     </row>
     <row r="224" spans="1:2">
       <c r="A224" s="1">
-        <v>42663</v>
+        <v>42367</v>
       </c>
       <c r="B224">
-        <v>0.7039404253165745</v>
+        <v>0.6878651725749189</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225" s="1">
-        <v>42411</v>
+        <v>43081</v>
       </c>
       <c r="B225">
-        <v>0.5885433800204616</v>
+        <v>0.6362277810902403</v>
       </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226" s="1">
-        <v>42180</v>
+        <v>42675</v>
       </c>
       <c r="B226">
-        <v>0.5294593417374607</v>
+        <v>0.6510428782841101</v>
       </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227" s="1">
-        <v>43048</v>
+        <v>42451</v>
       </c>
       <c r="B227">
-        <v>0.5586514727641088</v>
+        <v>0.6395307184192111</v>
       </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228" s="1">
-        <v>42271</v>
+        <v>41576</v>
       </c>
       <c r="B228">
-        <v>0.6289543740659138</v>
+        <v>0.5891765793796149</v>
       </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229" s="1">
-        <v>43062</v>
+        <v>41436</v>
       </c>
       <c r="B229">
-        <v>0.5966841463497148</v>
+        <v>0.681425500430809</v>
       </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230" s="1">
-        <v>41970</v>
+        <v>41807</v>
       </c>
       <c r="B230">
-        <v>0.7218596528130886</v>
+        <v>0.7758022211231016</v>
       </c>
     </row>
     <row r="231" spans="1:2">
       <c r="A231" s="1">
-        <v>42775</v>
+        <v>42255</v>
       </c>
       <c r="B231">
-        <v>0.5763288993561763</v>
+        <v>0.6451750287824872</v>
       </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232" s="1">
-        <v>43111</v>
+        <v>41779</v>
       </c>
       <c r="B232">
-        <v>0.641811448046131</v>
+        <v>0.7235117857089505</v>
       </c>
     </row>
     <row r="233" spans="1:2">
       <c r="A233" s="1">
-        <v>43216</v>
+        <v>43025</v>
       </c>
       <c r="B233">
-        <v>0.6490691281986285</v>
+        <v>0.688858112544122</v>
       </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234" s="1">
-        <v>42712</v>
+        <v>42388</v>
       </c>
       <c r="B234">
-        <v>0.6653438171794881</v>
+        <v>0.6473397857217597</v>
       </c>
     </row>
     <row r="235" spans="1:2">
       <c r="A235" s="1">
-        <v>43363</v>
+        <v>42297</v>
       </c>
       <c r="B235">
-        <v>0.6955841211726738</v>
+        <v>0.6752638197016664</v>
       </c>
     </row>
     <row r="236" spans="1:2">
       <c r="A236" s="1">
-        <v>42285</v>
+        <v>41828</v>
       </c>
       <c r="B236">
-        <v>0.7517693778603886</v>
+        <v>0.5940301995864897</v>
       </c>
     </row>
     <row r="237" spans="1:2">
       <c r="A237" s="1">
-        <v>42887</v>
+        <v>42283</v>
       </c>
       <c r="B237">
-        <v>0.6522586374472567</v>
+        <v>0.6653547093145722</v>
       </c>
     </row>
     <row r="238" spans="1:2">
       <c r="A238" s="1">
-        <v>42789</v>
+        <v>42899</v>
       </c>
       <c r="B238">
-        <v>0.5500941448141663</v>
+        <v>0.6412440347775037</v>
       </c>
     </row>
     <row r="239" spans="1:2">
       <c r="A239" s="1">
-        <v>42474</v>
+        <v>42654</v>
       </c>
       <c r="B239">
-        <v>0.6889175997124533</v>
+        <v>0.6255168220090302</v>
       </c>
     </row>
     <row r="240" spans="1:2">
       <c r="A240" s="1">
-        <v>42523</v>
+        <v>42766</v>
       </c>
       <c r="B240">
-        <v>0.6264935262799276</v>
+        <v>0.546309531996694</v>
       </c>
     </row>
     <row r="241" spans="1:2">
       <c r="A241" s="1">
-        <v>41592</v>
+        <v>41624</v>
       </c>
       <c r="B241">
-        <v>0.6899992820424832</v>
+        <v>0.7662162545435328</v>
       </c>
     </row>
     <row r="242" spans="1:2">
       <c r="A242" s="1">
-        <v>42817</v>
+        <v>41618</v>
       </c>
       <c r="B242">
-        <v>0.667926226787024</v>
+        <v>0.7467138969678879</v>
       </c>
     </row>
     <row r="243" spans="1:2">
       <c r="A243" s="1">
-        <v>42376</v>
+        <v>43039</v>
       </c>
       <c r="B243">
-        <v>0.678399249459988</v>
+        <v>0.67681990159216</v>
       </c>
     </row>
     <row r="244" spans="1:2">
       <c r="A244" s="1">
-        <v>42082</v>
+        <v>41863</v>
       </c>
       <c r="B244">
-        <v>0.6925561652614839</v>
+        <v>0.5538027284959711</v>
       </c>
     </row>
     <row r="245" spans="1:2">
       <c r="A245" s="1">
-        <v>41942</v>
+        <v>42073</v>
       </c>
       <c r="B245">
-        <v>0.712558180797827</v>
+        <v>0.6146146961908522</v>
       </c>
     </row>
     <row r="246" spans="1:2">
       <c r="A246" s="1">
-        <v>43314</v>
+        <v>42486</v>
       </c>
       <c r="B246">
-        <v>0.5710675089775544</v>
+        <v>0.606392610525103</v>
       </c>
     </row>
     <row r="247" spans="1:2">
       <c r="A247" s="1">
-        <v>42838</v>
+        <v>42409</v>
       </c>
       <c r="B247">
-        <v>0.6803144728914048</v>
+        <v>0.671199683241266</v>
       </c>
     </row>
     <row r="248" spans="1:2">
       <c r="A248" s="1">
-        <v>42908</v>
+        <v>42619</v>
       </c>
       <c r="B248">
-        <v>0.7061324657494804</v>
+        <v>0.5750443038859435</v>
       </c>
     </row>
     <row r="249" spans="1:2">
       <c r="A249" s="1">
-        <v>43328</v>
+        <v>42052</v>
       </c>
       <c r="B249">
-        <v>0.586418807041611</v>
+        <v>0.6458349674083042</v>
       </c>
     </row>
     <row r="250" spans="1:2">
       <c r="A250" s="1">
-        <v>43097</v>
+        <v>42990</v>
       </c>
       <c r="B250">
-        <v>0.564103747176483</v>
+        <v>0.6372479695597465</v>
       </c>
     </row>
     <row r="251" spans="1:2">
       <c r="A251" s="1">
-        <v>42306</v>
+        <v>42031</v>
       </c>
       <c r="B251">
-        <v>0.8294428715812254</v>
+        <v>0.6492791626004607</v>
       </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252" s="1">
-        <v>42691</v>
+        <v>42003</v>
       </c>
       <c r="B252">
-        <v>0.5943292757126705</v>
+        <v>0.517423470738716</v>
       </c>
     </row>
     <row r="253" spans="1:2">
       <c r="A253" s="1">
-        <v>43230</v>
+        <v>42584</v>
       </c>
       <c r="B253">
-        <v>0.7397655418233707</v>
+        <v>0.5992173850786541</v>
       </c>
     </row>
     <row r="254" spans="1:2">
       <c r="A254" s="1">
-        <v>43069</v>
+        <v>42976</v>
       </c>
       <c r="B254">
-        <v>0.5627523214339655</v>
+        <v>0.5015741537649527</v>
       </c>
     </row>
     <row r="255" spans="1:2">
       <c r="A255" s="1">
-        <v>41893</v>
+        <v>41814</v>
       </c>
       <c r="B255">
-        <v>0.6410209689651514</v>
+        <v>0.7431724685464136</v>
       </c>
     </row>
     <row r="256" spans="1:2">
       <c r="A256" s="1">
-        <v>42278</v>
+        <v>42311</v>
       </c>
       <c r="B256">
-        <v>0.6716436205055114</v>
+        <v>0.7150244239779453</v>
       </c>
     </row>
     <row r="257" spans="1:2">
       <c r="A257" s="1">
-        <v>42894</v>
+        <v>42164</v>
       </c>
       <c r="B257">
-        <v>0.5889334836011495</v>
+        <v>0.7065841819889814</v>
       </c>
     </row>
     <row r="258" spans="1:2">
       <c r="A258" s="1">
-        <v>43104</v>
+        <v>42780</v>
       </c>
       <c r="B258">
-        <v>0.55472748621811</v>
+        <v>0.583975122947777</v>
       </c>
     </row>
     <row r="259" spans="1:2">
       <c r="A259" s="1">
-        <v>41648</v>
+        <v>43046</v>
       </c>
       <c r="B259">
-        <v>0.6174547702210406</v>
+        <v>0.6111114811371945</v>
       </c>
     </row>
     <row r="260" spans="1:2">
       <c r="A260" s="1">
-        <v>42922</v>
+        <v>42885</v>
       </c>
       <c r="B260">
-        <v>0.6647951424355724</v>
+        <v>0.6372801911851695</v>
       </c>
     </row>
     <row r="261" spans="1:2">
       <c r="A261" s="1">
-        <v>41844</v>
+        <v>42248</v>
       </c>
       <c r="B261">
-        <v>0.6384964827938558</v>
+        <v>0.7014891678608055</v>
       </c>
     </row>
     <row r="262" spans="1:2">
       <c r="A262" s="1">
-        <v>43174</v>
+        <v>42234</v>
       </c>
       <c r="B262">
-        <v>0.6576285305869662</v>
+        <v>0.6236745473184504</v>
       </c>
     </row>
   </sheetData>

</xml_diff>